<commit_message>
Update raw files and create models
</commit_message>
<xml_diff>
--- a/Chlorophyll.xlsx
+++ b/Chlorophyll.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\St Andrews Academic\PhD\Projects\MicroBE\2019 Analysis\Reorganised stats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\St Andrews Academic\PhD\Projects\MicroBE\Manuscript\Supplemantary materials\GitHub\ASSEMBLE-MICROBE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B119FB6-2AC9-4955-9998-BA2C7254C0C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183E18FF-6483-44B6-93C0-2112E5C6410C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F6ED0E85-F02E-49BF-AB9B-A599AF36116E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F6ED0E85-F02E-49BF-AB9B-A599AF36116E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
     <t>Control</t>
   </si>
   <si>
-    <t>Chlorophyll (μg g-1 dry sediment)</t>
+    <t>Chlorophyll</t>
   </si>
 </sst>
 </file>
@@ -406,7 +406,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>